<commit_message>
Rule Proc Table/Trikramam for Raja 26/0/92020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Trikrama Table.xlsx
+++ b/TS Jatai Working/Raja Files/Trikrama Table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t xml:space="preserve">Trikrama Table </t>
   </si>
@@ -168,9 +168,6 @@
     <t>vRuqkShiq</t>
   </si>
   <si>
-    <t>uqtyA</t>
-  </si>
-  <si>
     <t>BUqtvA</t>
   </si>
   <si>
@@ -217,6 +214,21 @@
   </si>
   <si>
     <t>nAka$m</t>
+  </si>
+  <si>
+    <t>1.5.1.3</t>
+  </si>
+  <si>
+    <t>tvaShTA$</t>
+  </si>
+  <si>
+    <t>dhAqtA</t>
+  </si>
+  <si>
+    <t>UqtyA</t>
+  </si>
+  <si>
+    <t>1.6.6.1</t>
   </si>
 </sst>
 </file>
@@ -289,12 +301,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,18 +627,18 @@
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -642,7 +655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -663,7 +676,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>+A5+1</f>
         <v>2</v>
@@ -685,16 +698,16 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" ref="A7:A25" si="0">+A6+1</f>
+        <f t="shared" ref="A7:A27" si="0">+A6+1</f>
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -707,198 +720,201 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="C10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -911,19 +927,19 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -933,16 +949,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>53</v>
+      <c r="E18" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
@@ -955,19 +971,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -977,16 +993,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -999,16 +1015,16 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>8</v>
@@ -1021,20 +1037,21 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -1042,20 +1059,21 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -1063,16 +1081,16 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
@@ -1084,18 +1102,60 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>